<commit_message>
Updated Sprint12 stand-up meeting templet.
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint12/Team05 Stand-up Meeting Sprint12.xlsx
+++ b/Project_Files/Sprint12/Team05 Stand-up Meeting Sprint12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s546942\Dropbox\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint12\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859AB350-E532-4C3F-99DF-7A21A9E62AF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6CB450-E6EC-46F7-A5C7-81E3B615E2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="760" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <r>
       <rPr>
@@ -136,12 +136,30 @@
 2.What will I do today?
 3.What obstacles are impeding my progress?</t>
   </si>
+  <si>
+    <t>I have modified backedcode on event page and update event using recycler view, intents.</t>
+  </si>
+  <si>
+    <t>We are successful in fixing the issue with menu item selection.</t>
+  </si>
+  <si>
+    <t>Added Event Date search Functionality</t>
+  </si>
+  <si>
+    <t>I will work on minor enhancement like date search and event search functionality</t>
+  </si>
+  <si>
+    <t>I need to work on date search functionality.</t>
+  </si>
+  <si>
+    <t>Need to fix issues</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +209,14 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF252525"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,8 +235,14 @@
         <bgColor theme="0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -427,11 +457,71 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -478,6 +568,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -696,8 +804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1071,7 +1179,7 @@
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
     </row>
-    <row r="13" spans="1:26" ht="13.5" customHeight="1">
+    <row r="13" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A13" s="11"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
@@ -1105,13 +1213,19 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="13.5" customHeight="1">
+    <row r="14" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A14" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="B14" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="28" t="s">
+        <v>22</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
@@ -1135,11 +1249,17 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="13.5" customHeight="1">
+    <row r="15" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A15" s="10"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="4"/>
+      <c r="B15" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>25</v>
+      </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1163,11 +1283,17 @@
       <c r="Y15" s="1"/>
       <c r="Z15" s="1"/>
     </row>
-    <row r="16" spans="1:26" ht="13.5" customHeight="1">
+    <row r="16" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A16" s="11"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="B16" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>7</v>
+      </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -28765,6 +28891,6 @@
     <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated daily standup meeting file
Updated daily objectives and completed objectives for the sprint 12
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint12/Team05 Stand-up Meeting Sprint12.xlsx
+++ b/Project_Files/Sprint12/Team05 Stand-up Meeting Sprint12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S547049\Documents\GitHub\FreebiesforNewbies\Project_Files\Sprint12\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/Sprint12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6CB450-E6EC-46F7-A5C7-81E3B615E2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{0A6CB450-E6EC-46F7-A5C7-81E3B615E2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE2464D6-EDAD-4BCA-A7BA-3C074D73A935}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="760" windowWidth="19180" windowHeight="9780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <r>
       <rPr>
@@ -153,6 +153,24 @@
   </si>
   <si>
     <t>Need to fix issues</t>
+  </si>
+  <si>
+    <t>Worked on date picker and no action bar for menu</t>
+  </si>
+  <si>
+    <t>I will work on home UI page to perform CRUD operations</t>
+  </si>
+  <si>
+    <t>Getting know about how to implement the CRUD operations for the UI part</t>
+  </si>
+  <si>
+    <t>Continue for learning about UI CRUD implemenatation parts</t>
+  </si>
+  <si>
+    <t>learning about UI CRUD implemenatation parts</t>
+  </si>
+  <si>
+    <t>implementing new things in UI</t>
   </si>
 </sst>
 </file>
@@ -539,6 +557,24 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -568,24 +604,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -804,8 +822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -816,12 +834,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A1" s="19"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="21"/>
+      <c r="A1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -844,12 +862,12 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A2" s="17"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="18"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -872,14 +890,14 @@
       <c r="Z2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="25"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -902,14 +920,14 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="25"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -932,14 +950,14 @@
       <c r="Z4" s="1"/>
     </row>
     <row r="5" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="25"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1024,7 +1042,7 @@
       <c r="Z7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="4"/>
@@ -1054,7 +1072,7 @@
       <c r="Z8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A9" s="10"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
@@ -1082,7 +1100,7 @@
       <c r="Z9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A10" s="11"/>
+      <c r="A10" s="17"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
@@ -1110,7 +1128,7 @@
       <c r="Z10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1146,7 +1164,7 @@
       <c r="Z11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A12" s="10"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1180,7 +1198,7 @@
       <c r="Z12" s="1"/>
     </row>
     <row r="13" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A13" s="11"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="5" t="s">
         <v>7</v>
       </c>
@@ -1214,16 +1232,16 @@
       <c r="Z13" s="1"/>
     </row>
     <row r="14" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="28" t="s">
+      <c r="D14" s="10" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="1"/>
@@ -1250,14 +1268,14 @@
       <c r="Z14" s="1"/>
     </row>
     <row r="15" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="29" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E15" s="1"/>
@@ -1284,14 +1302,14 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="32" t="s">
+      <c r="A16" s="17"/>
+      <c r="B16" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="31" t="s">
+      <c r="C16" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="13" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="1"/>
@@ -1318,12 +1336,18 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1348,10 +1372,16 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1376,10 +1406,16 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1404,7 +1440,7 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A20" s="12" t="s">
+      <c r="A20" s="18" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="4"/>
@@ -1434,7 +1470,7 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A21" s="10"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
@@ -1462,7 +1498,7 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A22" s="11"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
@@ -1576,10 +1612,10 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="14"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1606,8 +1642,8 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A27" s="15"/>
-      <c r="B27" s="16"/>
+      <c r="A27" s="21"/>
+      <c r="B27" s="22"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1634,8 +1670,8 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="13.5" customHeight="1">
-      <c r="A28" s="17"/>
-      <c r="B28" s="18"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>

</xml_diff>

<commit_message>
Updated Team Reports and other documents for the Client Team Meeting
</commit_message>
<xml_diff>
--- a/Project_Files/Sprint12/Team05 Stand-up Meeting Sprint12.xlsx
+++ b/Project_Files/Sprint12/Team05 Stand-up Meeting Sprint12.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546981_nwmissouri_edu/Documents/Documents/GitHub/FreebiesforNewbies/Project_Files/Sprint12/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nwmissouri-my.sharepoint.com/personal/s546907_nwmissouri_edu/Documents/Desktop/git-local-repo/FreebiesforNewbies/Project_Files/Sprint12/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{0A6CB450-E6EC-46F7-A5C7-81E3B615E2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE2464D6-EDAD-4BCA-A7BA-3C074D73A935}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{0A6CB450-E6EC-46F7-A5C7-81E3B615E2DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7F1690D-6148-4975-B63E-8C753CC1B8BB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -33,6 +33,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Week:</t>
     </r>
@@ -41,6 +42,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> Nov 14 - Nov 18</t>
     </r>
@@ -52,6 +54,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Project Name:</t>
     </r>
@@ -60,6 +63,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> Freebies for Newbies</t>
     </r>
@@ -71,6 +75,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t>Team Name:</t>
     </r>
@@ -79,6 +84,7 @@
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
+        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> 05</t>
     </r>
@@ -172,6 +178,27 @@
   <si>
     <t>implementing new things in UI</t>
   </si>
+  <si>
+    <t>I have worked on menu options for user to navigate between pages</t>
+  </si>
+  <si>
+    <t>We are successfull in fixing the issue with menu item selection.</t>
+  </si>
+  <si>
+    <t>Added search by name functionality in event home page</t>
+  </si>
+  <si>
+    <t>Need to work on fixings the issue.</t>
+  </si>
+  <si>
+    <t>I need to work on event search by name functionality.</t>
+  </si>
+  <si>
+    <t>Need to test the functionality.</t>
+  </si>
+  <si>
+    <t>App is not able to recognize selected menu Item id.</t>
+  </si>
 </sst>
 </file>
 
@@ -189,32 +216,38 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF252525"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -226,6 +259,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -539,8 +573,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="37">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -604,6 +638,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +869,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B8" sqref="B8:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -1007,7 +1053,7 @@
       <c r="Y6" s="1"/>
       <c r="Z6" s="1"/>
     </row>
-    <row r="7" spans="1:26" ht="13.5" customHeight="1">
+    <row r="7" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
         <v>3</v>
@@ -1041,13 +1087,19 @@
       <c r="Y7" s="1"/>
       <c r="Z7" s="1"/>
     </row>
-    <row r="8" spans="1:26" ht="13.5" customHeight="1">
+    <row r="8" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="B8" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="34" t="s">
+        <v>34</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1071,11 +1123,17 @@
       <c r="Y8" s="1"/>
       <c r="Z8" s="1"/>
     </row>
-    <row r="9" spans="1:26" ht="13.5" customHeight="1">
+    <row r="9" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A9" s="16"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="B9" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="36" t="s">
+        <v>37</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1099,11 +1157,17 @@
       <c r="Y9" s="1"/>
       <c r="Z9" s="1"/>
     </row>
-    <row r="10" spans="1:26" ht="13.5" customHeight="1">
+    <row r="10" spans="1:26" ht="13.5" customHeight="1" thickBot="1">
       <c r="A10" s="17"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="B10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>7</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>

</xml_diff>